<commit_message>
learning rates for part 4 updated as an array
</commit_message>
<xml_diff>
--- a/Networks/Parte4/Excel/Network16.xlsx
+++ b/Networks/Parte4/Excel/Network16.xlsx
@@ -524,52 +524,52 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-243.1939921186173</v>
+        <v>-80.43898936921897</v>
       </c>
       <c r="C2" t="n">
-        <v>-81.30094749596974</v>
+        <v>-84.59693280944545</v>
       </c>
       <c r="D2" t="n">
-        <v>-180.9990379920282</v>
+        <v>21.34236523684379</v>
       </c>
       <c r="E2" t="n">
-        <v>66.47060873810901</v>
+        <v>10.38196275134003</v>
       </c>
       <c r="F2" t="n">
-        <v>-81.38914818221747</v>
+        <v>-95.12887749917114</v>
       </c>
       <c r="G2" t="n">
-        <v>16.69341000807308</v>
+        <v>-92.19922354081878</v>
       </c>
       <c r="H2" t="n">
-        <v>101.8449389561158</v>
+        <v>26.32510524637755</v>
       </c>
       <c r="I2" t="n">
-        <v>84.40763551555976</v>
+        <v>-87.49995246128725</v>
       </c>
       <c r="J2" t="n">
-        <v>-200.7032067908499</v>
+        <v>-36.51126466649291</v>
       </c>
       <c r="K2" t="n">
-        <v>-239.6031066167007</v>
+        <v>41.22878403531359</v>
       </c>
       <c r="L2" t="n">
-        <v>146.0025018955688</v>
+        <v>-66.39558306760348</v>
       </c>
       <c r="M2" t="n">
-        <v>101.9121830324092</v>
+        <v>-35.82270513158981</v>
       </c>
       <c r="N2" t="n">
-        <v>-151.3686498915748</v>
+        <v>6.547334700058046</v>
       </c>
       <c r="O2" t="n">
-        <v>5.635390028382238</v>
+        <v>-57.86166776779288</v>
       </c>
       <c r="P2" t="n">
-        <v>-259.4556294321636</v>
+        <v>-5.303354547393592</v>
       </c>
       <c r="Q2" t="n">
-        <v>-246.8643984678709</v>
+        <v>25.49832450630915</v>
       </c>
     </row>
     <row r="3">
@@ -579,52 +579,52 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>113.6319220127359</v>
+        <v>36.12173736708888</v>
       </c>
       <c r="C3" t="n">
-        <v>119.6674536229856</v>
+        <v>36.6965667762617</v>
       </c>
       <c r="D3" t="n">
-        <v>83.14238006490058</v>
+        <v>-23.44653238773396</v>
       </c>
       <c r="E3" t="n">
-        <v>56.92100178758089</v>
+        <v>15.21481609898233</v>
       </c>
       <c r="F3" t="n">
-        <v>128.1607460927516</v>
+        <v>22.64823500236385</v>
       </c>
       <c r="G3" t="n">
-        <v>171.4109663068704</v>
+        <v>31.17960714002092</v>
       </c>
       <c r="H3" t="n">
-        <v>129.2003996650804</v>
+        <v>37.55553220181722</v>
       </c>
       <c r="I3" t="n">
-        <v>58.50476529219119</v>
+        <v>24.69445985098462</v>
       </c>
       <c r="J3" t="n">
-        <v>112.197919324819</v>
+        <v>37.65414465796103</v>
       </c>
       <c r="K3" t="n">
-        <v>64.96024009533195</v>
+        <v>34.72733634546212</v>
       </c>
       <c r="L3" t="n">
-        <v>104.7653737607316</v>
+        <v>40.08828477343197</v>
       </c>
       <c r="M3" t="n">
-        <v>-83.09910869998495</v>
+        <v>50.9459639680981</v>
       </c>
       <c r="N3" t="n">
-        <v>131.1186705829199</v>
+        <v>52.17678629191545</v>
       </c>
       <c r="O3" t="n">
-        <v>121.2680636650181</v>
+        <v>48.27450336493471</v>
       </c>
       <c r="P3" t="n">
-        <v>64.39915265898586</v>
+        <v>48.04927139684878</v>
       </c>
       <c r="Q3" t="n">
-        <v>79.77513112721221</v>
+        <v>24.83091110107623</v>
       </c>
     </row>
     <row r="4">
@@ -634,52 +634,52 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>86.81811540575269</v>
+        <v>31.93669440890826</v>
       </c>
       <c r="C4" t="n">
-        <v>28.13002774007484</v>
+        <v>27.42958055239869</v>
       </c>
       <c r="D4" t="n">
-        <v>60.39618540557586</v>
+        <v>22.98535237417797</v>
       </c>
       <c r="E4" t="n">
-        <v>2.907015918497961</v>
+        <v>5.474406718883306</v>
       </c>
       <c r="F4" t="n">
-        <v>120.0480845388575</v>
+        <v>23.76700586937886</v>
       </c>
       <c r="G4" t="n">
-        <v>4.93944801234199</v>
+        <v>27.11280669802687</v>
       </c>
       <c r="H4" t="n">
-        <v>-13.33194352916146</v>
+        <v>-0.5426471678387098</v>
       </c>
       <c r="I4" t="n">
-        <v>109.7717961123744</v>
+        <v>23.87075216396777</v>
       </c>
       <c r="J4" t="n">
-        <v>102.3713184613232</v>
+        <v>12.55619769111444</v>
       </c>
       <c r="K4" t="n">
-        <v>54.80396990263039</v>
+        <v>-3.92277470880153</v>
       </c>
       <c r="L4" t="n">
-        <v>-8.632618097190955</v>
+        <v>30.63898971081599</v>
       </c>
       <c r="M4" t="n">
-        <v>92.12903061158782</v>
+        <v>43.52161071855134</v>
       </c>
       <c r="N4" t="n">
-        <v>108.8919848257689</v>
+        <v>1.316285222177179</v>
       </c>
       <c r="O4" t="n">
-        <v>112.8494175487239</v>
+        <v>40.02004666684572</v>
       </c>
       <c r="P4" t="n">
-        <v>60.16204154303793</v>
+        <v>40.75862693202311</v>
       </c>
       <c r="Q4" t="n">
-        <v>69.14370838050482</v>
+        <v>38.31820406273182</v>
       </c>
     </row>
     <row r="5">
@@ -689,52 +689,52 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>37.33970044680822</v>
+        <v>10.84838020883303</v>
       </c>
       <c r="C5" t="n">
-        <v>105.8767028341903</v>
+        <v>18.39450958226062</v>
       </c>
       <c r="D5" t="n">
-        <v>47.08830341561317</v>
+        <v>5.964016709850147</v>
       </c>
       <c r="E5" t="n">
-        <v>93.59233344982236</v>
+        <v>23.9704887004397</v>
       </c>
       <c r="F5" t="n">
-        <v>28.11238677540703</v>
+        <v>16.49886809624139</v>
       </c>
       <c r="G5" t="n">
-        <v>0.8325292616237553</v>
+        <v>16.20013579152447</v>
       </c>
       <c r="H5" t="n">
-        <v>2.217363088962681</v>
+        <v>2.767597077344891</v>
       </c>
       <c r="I5" t="n">
-        <v>11.18402384897622</v>
+        <v>12.35497611026126</v>
       </c>
       <c r="J5" t="n">
-        <v>41.44191902213637</v>
+        <v>26.56690539195412</v>
       </c>
       <c r="K5" t="n">
-        <v>48.53281636394871</v>
+        <v>1.480528378347572</v>
       </c>
       <c r="L5" t="n">
-        <v>-10.0585884040484</v>
+        <v>14.47997330266823</v>
       </c>
       <c r="M5" t="n">
-        <v>14.88436247832616</v>
+        <v>14.193358526084</v>
       </c>
       <c r="N5" t="n">
-        <v>44.89994228350574</v>
+        <v>9.232601559639386</v>
       </c>
       <c r="O5" t="n">
-        <v>16.74658281456966</v>
+        <v>13.45533195688077</v>
       </c>
       <c r="P5" t="n">
-        <v>29.14513131130226</v>
+        <v>4.506013323324806</v>
       </c>
       <c r="Q5" t="n">
-        <v>55.50385203414432</v>
+        <v>0.9495051997838768</v>
       </c>
     </row>
     <row r="6">
@@ -744,52 +744,52 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>30.71402753062653</v>
+        <v>2.40863374808568</v>
       </c>
       <c r="C6" t="n">
-        <v>33.78460257228782</v>
+        <v>16.53777520442131</v>
       </c>
       <c r="D6" t="n">
-        <v>30.20333968747974</v>
+        <v>0.7189910774185907</v>
       </c>
       <c r="E6" t="n">
-        <v>51.71956793103686</v>
+        <v>14.58348644402134</v>
       </c>
       <c r="F6" t="n">
-        <v>25.19994864718893</v>
+        <v>8.721856521101261</v>
       </c>
       <c r="G6" t="n">
-        <v>9.778087468236032</v>
+        <v>16.42272544058079</v>
       </c>
       <c r="H6" t="n">
-        <v>4.401552600219372</v>
+        <v>2.485669232755435</v>
       </c>
       <c r="I6" t="n">
-        <v>0.2410845010952696</v>
+        <v>12.21574172971754</v>
       </c>
       <c r="J6" t="n">
-        <v>15.88501938413959</v>
+        <v>19.31443802007323</v>
       </c>
       <c r="K6" t="n">
-        <v>29.50388027570528</v>
+        <v>1.495710335843043</v>
       </c>
       <c r="L6" t="n">
-        <v>-2.082729104739657</v>
+        <v>10.79192134704409</v>
       </c>
       <c r="M6" t="n">
-        <v>15.34061134369629</v>
+        <v>8.638529127920561</v>
       </c>
       <c r="N6" t="n">
-        <v>34.96449189011512</v>
+        <v>6.238474256616009</v>
       </c>
       <c r="O6" t="n">
-        <v>23.39425956166872</v>
+        <v>7.889235635674853</v>
       </c>
       <c r="P6" t="n">
-        <v>25.19671158318345</v>
+        <v>6.787766561437699</v>
       </c>
       <c r="Q6" t="n">
-        <v>30.61937460147919</v>
+        <v>-4.921624540120979</v>
       </c>
     </row>
     <row r="7">
@@ -799,52 +799,52 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>13.54439782395952</v>
+        <v>1.386852788308471</v>
       </c>
       <c r="C7" t="n">
-        <v>1.10689806388691</v>
+        <v>1.674038817980375</v>
       </c>
       <c r="D7" t="n">
-        <v>1.3424733521879</v>
+        <v>3.310216006770275</v>
       </c>
       <c r="E7" t="n">
-        <v>2.256450641510126</v>
+        <v>4.819300480219698</v>
       </c>
       <c r="F7" t="n">
-        <v>5.170014805481797</v>
+        <v>0.9248943133802958</v>
       </c>
       <c r="G7" t="n">
-        <v>5.153751885278444</v>
+        <v>2.024029031774504</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.1952483185895791</v>
+        <v>-0.1502223852548318</v>
       </c>
       <c r="I7" t="n">
-        <v>7.703054713055342</v>
+        <v>2.83263571191881</v>
       </c>
       <c r="J7" t="n">
-        <v>1.852958402916555</v>
+        <v>3.296912335015902</v>
       </c>
       <c r="K7" t="n">
-        <v>3.546317906875929</v>
+        <v>0.03610241284409525</v>
       </c>
       <c r="L7" t="n">
-        <v>-3.857065036477403</v>
+        <v>2.249625007395552</v>
       </c>
       <c r="M7" t="n">
-        <v>1.069174568131278</v>
+        <v>2.414590305445437</v>
       </c>
       <c r="N7" t="n">
-        <v>6.993456079379818</v>
+        <v>-1.382018293644014</v>
       </c>
       <c r="O7" t="n">
-        <v>17.11243627858237</v>
+        <v>1.467238525330903</v>
       </c>
       <c r="P7" t="n">
-        <v>4.941594296467014</v>
+        <v>0.5226543081061649</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.7949896318884241</v>
+        <v>0.3310723279829608</v>
       </c>
     </row>
     <row r="8">
@@ -854,52 +854,52 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>27.49453891700169</v>
+        <v>0.234886022788448</v>
       </c>
       <c r="C8" t="n">
-        <v>4.398413883795521</v>
+        <v>2.307973429121319</v>
       </c>
       <c r="D8" t="n">
-        <v>-10.79123611725882</v>
+        <v>-1.30811233217117</v>
       </c>
       <c r="E8" t="n">
-        <v>7.42258916920427</v>
+        <v>0.5616666195211862</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.2666211815236582</v>
+        <v>1.965838236257432</v>
       </c>
       <c r="G8" t="n">
-        <v>-2.344030977188412</v>
+        <v>1.985181297714537</v>
       </c>
       <c r="H8" t="n">
-        <v>-2.468803116819266</v>
+        <v>0.69750481803818</v>
       </c>
       <c r="I8" t="n">
-        <v>0.4649001073531859</v>
+        <v>-0.487758710887738</v>
       </c>
       <c r="J8" t="n">
-        <v>5.013303480723808</v>
+        <v>4.688530991267798</v>
       </c>
       <c r="K8" t="n">
-        <v>0.7179538447214361</v>
+        <v>-0.123269317262097</v>
       </c>
       <c r="L8" t="n">
-        <v>0.8746506115345071</v>
+        <v>2.13186204198269</v>
       </c>
       <c r="M8" t="n">
-        <v>5.344969558420969</v>
+        <v>-1.003966738577074</v>
       </c>
       <c r="N8" t="n">
-        <v>4.654783639875077</v>
+        <v>2.106026688975086</v>
       </c>
       <c r="O8" t="n">
-        <v>1.498033322563415</v>
+        <v>0.8787126322624352</v>
       </c>
       <c r="P8" t="n">
-        <v>13.2819082441379</v>
+        <v>-0.6086727745488361</v>
       </c>
       <c r="Q8" t="n">
-        <v>1.868620683636425</v>
+        <v>1.844944573837262</v>
       </c>
     </row>
     <row r="9">
@@ -909,52 +909,52 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>5.045418358254545</v>
+        <v>0.5875991551779893</v>
       </c>
       <c r="C9" t="n">
-        <v>-3.115386273647082</v>
+        <v>1.229408458289134</v>
       </c>
       <c r="D9" t="n">
-        <v>-1.036611001926858</v>
+        <v>-0.6809125198675811</v>
       </c>
       <c r="E9" t="n">
-        <v>0.5008784718398032</v>
+        <v>-1.046585594789087</v>
       </c>
       <c r="F9" t="n">
-        <v>3.085609098881468</v>
+        <v>1.297238711683581</v>
       </c>
       <c r="G9" t="n">
-        <v>5.96087427145964</v>
+        <v>1.929372806937975</v>
       </c>
       <c r="H9" t="n">
-        <v>-2.507416252114525</v>
+        <v>-0.1446273075641309</v>
       </c>
       <c r="I9" t="n">
-        <v>0.2076050359171674</v>
+        <v>2.026026573466379</v>
       </c>
       <c r="J9" t="n">
-        <v>5.224914790634967</v>
+        <v>-3.200875860748735</v>
       </c>
       <c r="K9" t="n">
-        <v>1.141285177903672</v>
+        <v>0.5468405783365957</v>
       </c>
       <c r="L9" t="n">
-        <v>2.612607805262336</v>
+        <v>1.338712719398873</v>
       </c>
       <c r="M9" t="n">
-        <v>0.209680291252908</v>
+        <v>1.96868303023525</v>
       </c>
       <c r="N9" t="n">
-        <v>0.8047079318621791</v>
+        <v>1.292456659416576</v>
       </c>
       <c r="O9" t="n">
-        <v>3.381031899028428</v>
+        <v>4.18929850050441</v>
       </c>
       <c r="P9" t="n">
-        <v>18.68647604041724</v>
+        <v>3.080578912428321</v>
       </c>
       <c r="Q9" t="n">
-        <v>-4.325124028871036</v>
+        <v>1.66130742878565</v>
       </c>
     </row>
   </sheetData>
@@ -990,7 +990,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-275.2459096310733</v>
+        <v>-130.5267979698347</v>
       </c>
     </row>
     <row r="3">
@@ -1000,7 +1000,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>281.0554838617188</v>
+        <v>237.3162127402424</v>
       </c>
     </row>
     <row r="4">
@@ -1010,7 +1010,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>148.3407848566225</v>
+        <v>241.0222913309289</v>
       </c>
     </row>
     <row r="5">
@@ -1020,7 +1020,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>219.1854270122569</v>
+        <v>198.2821385838752</v>
       </c>
     </row>
     <row r="6">
@@ -1030,7 +1030,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>147.8264145572918</v>
+        <v>148.1299780180685</v>
       </c>
     </row>
     <row r="7">
@@ -1040,7 +1040,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>227.8431875601237</v>
+        <v>255.1211460002976</v>
       </c>
     </row>
     <row r="8">
@@ -1050,7 +1050,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>211.4306947541517</v>
+        <v>253.0847800494708</v>
       </c>
     </row>
     <row r="9">
@@ -1060,7 +1060,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>242.6551304195584</v>
+        <v>206.8081961141725</v>
       </c>
     </row>
     <row r="10">
@@ -1070,7 +1070,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>187.9141627353605</v>
+        <v>239.7413955284346</v>
       </c>
     </row>
     <row r="11">
@@ -1080,7 +1080,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>239.6772389256476</v>
+        <v>189.5307542810294</v>
       </c>
     </row>
     <row r="12">
@@ -1090,7 +1090,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>280.5885602666945</v>
+        <v>217.9731197395053</v>
       </c>
     </row>
     <row r="13">
@@ -1100,7 +1100,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>253.9903492090896</v>
+        <v>237.0091498950191</v>
       </c>
     </row>
     <row r="14">
@@ -1110,7 +1110,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>194.7944831959388</v>
+        <v>219.0983079764121</v>
       </c>
     </row>
     <row r="15">
@@ -1120,7 +1120,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>256.0692776521478</v>
+        <v>187.4066649630552</v>
       </c>
     </row>
     <row r="16">
@@ -1130,7 +1130,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>204.013445797989</v>
+        <v>236.6716639065425</v>
       </c>
     </row>
     <row r="17">
@@ -1140,7 +1140,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>297.3882677910987</v>
+        <v>204.0489046305277</v>
       </c>
     </row>
     <row r="18">
@@ -1150,7 +1150,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>292.6068390368043</v>
+        <v>183.5250503332178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>